<commit_message>
Update operating range diagram.
</commit_message>
<xml_diff>
--- a/Paper/fig/rough-work-III.xlsx
+++ b/Paper/fig/rough-work-III.xlsx
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="53">
   <si>
     <t>CondTemp</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>-&gt; in Celsius</t>
+  </si>
+  <si>
+    <t>Operating range (Map 6)</t>
   </si>
 </sst>
 </file>
@@ -14279,7 +14282,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Operating Range</c:v>
+            <c:v>Operating Range (Map 6)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -33339,7 +33342,7 @@
   <dimension ref="A1:R212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T73" sqref="T73"/>
+      <selection activeCell="AH76" sqref="AH76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33349,7 +33352,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>

</xml_diff>